<commit_message>
Update diseases templates to deal with general question
</commit_message>
<xml_diff>
--- a/src/main/groovy/projects/gecco/crf/GroovyGenerator/Anamnesis/Diseases/values_RheumaImunoDiseases.xlsx
+++ b/src/main/groovy/projects/gecco/crf/GroovyGenerator/Anamnesis/Diseases/values_RheumaImunoDiseases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\IdeaProjects\kairos-fhir-dsl-mapping-example\src\main\groovy\projects\gecco\crf\GroovyGeneratorFromTemplate\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mario Macedo\IdeaProjects\kairos-fhir-dsl-mapping-example\src\main\groovy\projects\gecco\crf\GroovyGenerator\Anamnesis\Diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F40347F-2052-4799-88A5-941D5C452275}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8126E9-9CD8-4D97-AA7B-9E72ADDC20CA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,54 +31,36 @@
     <t>Rheumatoide Arthritis</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_RHEUMATOIDE_ARTHRITIS</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an rheumatoider Arthritis?</t>
   </si>
   <si>
     <t>Kollagenosen</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_KOLLAGENOSEN</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an Kollagenosen?</t>
   </si>
   <si>
     <t>Vaskulitis</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_VASKULITIS</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an Vaskulitis?</t>
   </si>
   <si>
     <t>angeborene Immundefekte</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_ANGEBORENE_IMMUNDEFEKTE</t>
-  </si>
-  <si>
     <t>Hat der/die Patient*in angeborene Immundefekte?</t>
   </si>
   <si>
     <t>Rheumatologische Erkrankung</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_RHEUMATOLOGISCHE_ERKRANKUNG</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an rheumatologischen Erkrankungen?</t>
   </si>
   <si>
     <t>Immunologische Erkrankung</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_IMMUNOLOGISCHE_ERKRANKUNG</t>
-  </si>
-  <si>
     <t>Leidet der/die Patient*in an einer immunologischen Erkrankung?</t>
   </si>
   <si>
@@ -148,7 +130,25 @@
     <t>Chronisch entzuendliche Darmerkrankung</t>
   </si>
   <si>
-    <t>COV_GECCO_IMMONOLOGISCHE_ERKRANKUNG_CHRONISCH_ENTZUENDLICHE_DARMERKRANKUNG</t>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_CHRONISCH_ENTZUENDLICHE_DARMERKRANKUNG</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_RHEUMATOIDE_ARTHRITIS</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_KOLLAGENOSEN</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_VASKULITIS</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_ANGEBORENE_IMMUNDEFEKTE</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_RHEUMATOLOGISCHE_ERKRANKUNG</t>
+  </si>
+  <si>
+    <t>COV_GECCO_IMMUNOLOGISCHE_ERKRANKUNG_IMMUNOLOGISCHE_ERKRANKUNG</t>
   </si>
 </sst>
 </file>
@@ -1510,7 +1510,7 @@
   <dimension ref="A1:K61"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1531,25 +1531,25 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E1" s="11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>32</v>
       </c>
       <c r="H1" s="11"/>
       <c r="I1" s="11"/>
@@ -1557,20 +1557,20 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="D2" s="11"/>
       <c r="E2" s="11">
         <v>24526004</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>0</v>
@@ -1582,25 +1582,25 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E3" s="11">
         <v>69896004</v>
       </c>
       <c r="F3" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="11" t="s">
         <v>2</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>3</v>
       </c>
       <c r="H3" s="11"/>
       <c r="I3" s="11"/>
@@ -1609,25 +1609,25 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E4" s="11">
         <v>105969002</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H4" s="11"/>
       <c r="I4" s="11"/>
@@ -1636,23 +1636,23 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="11"/>
       <c r="E5" s="11">
         <v>31996006</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="G5" s="11" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
@@ -1661,23 +1661,23 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="11">
         <v>36138009</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="G6" s="11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H6" s="11"/>
       <c r="I6" s="11"/>
@@ -1686,23 +1686,23 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D7" s="11"/>
       <c r="E7" s="11">
         <v>396332003</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="G7" s="11" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="11"/>
@@ -1711,23 +1711,23 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D8" s="11"/>
       <c r="E8" s="11">
         <v>414029004</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11"/>

</xml_diff>